<commit_message>
Added agenda points and the retrospective for sprint 2
</commit_message>
<xml_diff>
--- a/doc/sprint2/retrospective.xlsx
+++ b/doc/sprint2/retrospective.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomw\Documents\Github\template\doc\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01CAD59-C39E-488E-BE75-7DBFE4B21322}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AE4E76-3F9B-4BE9-8B55-6E36391C0327}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16260" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Retrospective" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Sprint Retrospective</t>
   </si>
   <si>
     <t>Iteration</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
   </si>
   <si>
     <t>Project</t>
@@ -77,6 +74,105 @@
   </si>
   <si>
     <t>Adjustments for next Sprint Plan</t>
+  </si>
+  <si>
+    <t>Max and Thom</t>
+  </si>
+  <si>
+    <t>Dan Dan and Jason</t>
+  </si>
+  <si>
+    <t>Work had to be redone after Sander's memo</t>
+  </si>
+  <si>
+    <t>Work had to be redone after Sander's memo. Also, it was mostly Max and Dan Dan working on the code as Thom moved on to organising the directory and deliverables.</t>
+  </si>
+  <si>
+    <t>Thom</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Mostly</t>
+  </si>
+  <si>
+    <t>Make basic client</t>
+  </si>
+  <si>
+    <t>Make basic server</t>
+  </si>
+  <si>
+    <t>Design GUI</t>
+  </si>
+  <si>
+    <t>Harshitaa</t>
+  </si>
+  <si>
+    <t>Git issues</t>
+  </si>
+  <si>
+    <t>Various git-related misconfigurations and ghost branches that kept rearing their ugly heads did slow our progress.</t>
+  </si>
+  <si>
+    <t>Somewhere in the first halve of the week we decided on some conventions, mostly related to branching to keep our workflow professional</t>
+  </si>
+  <si>
+    <t>Broken Maven dependencies</t>
+  </si>
+  <si>
+    <t>Despite our best efforts to configure them neatly in Intellij, the dependencies were quite quirky.</t>
+  </si>
+  <si>
+    <t>We have not resolved this problem yet and will discuss this Monday if needed.</t>
+  </si>
+  <si>
+    <t>Implement basic GUI in JavaFX</t>
+  </si>
+  <si>
+    <t>Go Green</t>
+  </si>
+  <si>
+    <t>I as a user want my information to be fetched from the server</t>
+  </si>
+  <si>
+    <t>I as a user want to interact with the app using a simple UI</t>
+  </si>
+  <si>
+    <t>Organizing and working on paperwork</t>
+  </si>
+  <si>
+    <t>I as a developer want to organize the user data in a database</t>
+  </si>
+  <si>
+    <t>Make ER-schema for database</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>There was some doubt about what should go in the schema so work has not started</t>
+  </si>
+  <si>
+    <t>We will make sure that we know exactly what is expected from us so that we don't have to do things like rewriting socket networking code to use spring</t>
+  </si>
+  <si>
+    <t>Problem 3</t>
+  </si>
+  <si>
+    <t>Obligatory from sockets to spring</t>
+  </si>
+  <si>
+    <t>Though we thought we could just use sockets, a message from Sander revealed that we must use an api.</t>
+  </si>
+  <si>
+    <t>Though we wasted some time, we are now well on our way to developing a working spring client-server interaction</t>
+  </si>
+  <si>
+    <t>We will anticipate issues with technologies we are unfamiliar with, as a substantial amount of time was wasted on problems with git and maven.</t>
+  </si>
+  <si>
+    <t>I as a developer I want the paperwork to be straightforward and properly organized</t>
   </si>
 </sst>
 </file>
@@ -575,7 +671,9 @@
   </sheetPr>
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -620,7 +718,7 @@
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="8">
         <v>2</v>
       </c>
       <c r="E2" s="5"/>
@@ -677,9 +775,11 @@
     <row r="4" spans="1:26" ht="13.2">
       <c r="A4" s="1"/>
       <c r="B4" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="13"/>
@@ -707,9 +807,11 @@
     <row r="5" spans="1:26" ht="13.2">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="13"/>
@@ -793,25 +895,25 @@
     <row r="8" spans="1:26" ht="34.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="E8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="G8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -832,15 +934,29 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="13.2">
+    <row r="9" spans="1:26" ht="26.4">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -863,12 +979,24 @@
     <row r="10" spans="1:26" ht="13.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -888,14 +1016,26 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="13.2">
+    <row r="11" spans="1:26" ht="26.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -916,14 +1056,24 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="13.2">
+    <row r="12" spans="1:26" ht="26.4">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -944,17 +1094,25 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="45.6">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18" t="s">
-        <v>12</v>
+    <row r="13" spans="1:26" ht="39.6">
+      <c r="B13" s="2" t="s">
+        <v>50</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="17"/>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
+        <v>3</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -974,15 +1132,28 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="13.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="1"/>
+    <row r="14" spans="1:26" ht="26.4">
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1002,17 +1173,17 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="13.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="21" t="s">
-        <v>13</v>
+    <row r="15" spans="1:26" ht="45.6">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
+        <v>11</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="1"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1034,9 +1205,7 @@
     </row>
     <row r="16" spans="1:26" ht="13.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1064,10 +1233,12 @@
     </row>
     <row r="17" spans="1:26" ht="13.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="22" t="s">
-        <v>15</v>
+      <c r="B17" s="21" t="s">
+        <v>12</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
@@ -1092,10 +1263,14 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="13.2">
+    <row r="18" spans="1:26" ht="79.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
@@ -1120,12 +1295,14 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="13.2">
+    <row r="19" spans="1:26" ht="92.4">
       <c r="A19" s="1"/>
-      <c r="B19" s="21" t="s">
-        <v>16</v>
+      <c r="B19" s="22" t="s">
+        <v>14</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
@@ -1152,9 +1329,7 @@
     </row>
     <row r="20" spans="1:26" ht="13.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="B20" s="22"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1180,12 +1355,14 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="13.2">
+    <row r="21" spans="1:26" ht="26.4">
       <c r="A21" s="1"/>
-      <c r="B21" s="22" t="s">
-        <v>17</v>
+      <c r="B21" s="21" t="s">
+        <v>15</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
@@ -1210,10 +1387,14 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="13.2">
+    <row r="22" spans="1:26" ht="66">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="B22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
@@ -1238,10 +1419,14 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="13.2">
+    <row r="23" spans="1:26" ht="52.8">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
@@ -1266,17 +1451,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="45.6">
-      <c r="A24" s="17"/>
-      <c r="B24" s="18" t="s">
-        <v>18</v>
+    <row r="24" spans="1:26" ht="26.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="21" t="s">
+        <v>45</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="17"/>
+      <c r="C24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1296,10 +1483,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="13.2">
+    <row r="25" spans="1:26" ht="66">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
@@ -1324,15 +1515,13 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="13.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="1"/>
+    <row r="26" spans="1:26" ht="79.2">
+      <c r="B26" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1352,15 +1541,17 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="13.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="1"/>
+    <row r="27" spans="1:26" ht="45.6">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="17"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1380,10 +1571,12 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="13.2">
+    <row r="28" spans="1:26" ht="92.4">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
@@ -1408,10 +1601,12 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="13.2">
+    <row r="29" spans="1:26" ht="105.6">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
@@ -28373,27 +28568,27 @@
       <c r="Z991" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G991 F8 H8">
+  <conditionalFormatting sqref="F8 H8 G1:G25 G27:G991">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G991 F8 H8">
+  <conditionalFormatting sqref="F8 H8 G1:G25 G27:G991">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"B"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G991 F8 H8">
+  <conditionalFormatting sqref="F8 H8 G1:G25 G27:G991">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"C"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G991 F8 H8">
+  <conditionalFormatting sqref="F8 H8 G1:G25 G27:G991">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G991 F8 H8">
+  <conditionalFormatting sqref="F8 H8 G1:G25 G27:G991">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"E"</formula>
     </cfRule>

</xml_diff>